<commit_message>
uploading all file as backup plan before laptop dies....
</commit_message>
<xml_diff>
--- a/TestData/testData.xlsx
+++ b/TestData/testData.xlsx
@@ -62,7 +62,7 @@
     <t>zipCode</t>
   </si>
   <si>
-    <t>Neha</t>
+    <t>Nehaa</t>
   </si>
   <si>
     <t>Patni</t>
@@ -1227,7 +1227,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1"/>

</xml_diff>